<commit_message>
manual specialisations finished, but still has a bug, because always printing "Ta specjalizacja została już wybrana"
</commit_message>
<xml_diff>
--- a/Specjalizacje.xlsx
+++ b/Specjalizacje.xlsx
@@ -79,13 +79,13 @@
     <t xml:space="preserve">Bojka</t>
   </si>
   <si>
-    <t xml:space="preserve">refleks, walka wrecz, zmysl bojowy, ciche poruszanie, sprawnosc fizyczna, survival </t>
+    <t xml:space="preserve">refleks, walka wrecz, zmysl bitewny, ciche poruszanie, sprawnosc fizyczna, survival </t>
   </si>
   <si>
     <t xml:space="preserve">Eliminacja wrecz</t>
   </si>
   <si>
-    <t xml:space="preserve">refleks, walka wrecz, zmysł bojowy, ciche poruszanie, sprawnosc fizyczna, zreczne palce </t>
+    <t xml:space="preserve">refleks, walka wrecz, zmysł bitewny, ciche poruszanie, sprawnosc fizyczna, zreczne palce </t>
   </si>
   <si>
     <t xml:space="preserve">Tarcze</t>
@@ -273,7 +273,9 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -313,10 +315,10 @@
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="131.02"/>

</xml_diff>

<commit_message>
tests are suplemented, now all the scope is ready.
</commit_message>
<xml_diff>
--- a/Specjalizacje.xlsx
+++ b/Specjalizacje.xlsx
@@ -34,7 +34,7 @@
     <t xml:space="preserve">obsluga broni, refleks, strzelectwo, zmysl bitewny, spostrzeganie, sprawnosc fizyczna </t>
   </si>
   <si>
-    <t xml:space="preserve">Broń krotka</t>
+    <t xml:space="preserve">Bron krotka</t>
   </si>
   <si>
     <t xml:space="preserve">obsluga broni, refleks, strzelectwo, zmysl bitewny, ukrywanie, zreczne palce </t>
@@ -315,10 +315,10 @@
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="131.02"/>

</xml_diff>

<commit_message>
added predisposition, with tests.
</commit_message>
<xml_diff>
--- a/Specjalizacje.xlsx
+++ b/Specjalizacje.xlsx
@@ -314,7 +314,7 @@
   </sheetPr>
   <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -436,7 +436,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="8.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
Battle sence finally propered used.  next Languages.
</commit_message>
<xml_diff>
--- a/Specjalizacje.xlsx
+++ b/Specjalizacje.xlsx
@@ -20,7 +20,34 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="71">
+  <si>
+    <t xml:space="preserve">nazwa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">umiejętności powiązane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">umiejka1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">warunki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">opis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">umiejka2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">umiejka3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">umiejka4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ULT</t>
+  </si>
   <si>
     <t xml:space="preserve">Bron boczna</t>
   </si>
@@ -28,6 +55,53 @@
     <t xml:space="preserve">obsluga broni, refleks, strzelectwo, prowadzenie pojazdu, ukrywanie, zreczne palce </t>
   </si>
   <si>
+    <t xml:space="preserve">Wprawa
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pistolet, Rewolwer, Pistolet maszynowy, Jednoręczna, Kompaktowa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Możesz zamienić wynik wyrzucony na jednej z kości podczas testu Strzelectwa na liczbę równą poziomowi tej umiejętności podczas strzelania z broni z którąś z zasad Pistolet, Rewolwer, Pistolet maszynowy, Jednoręczna, Kompaktowa. Nie łączy się z umiejętnościami o tej samej nazwie z innych specjalizacji.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zasieg, Z biodra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pistolet, Rewolwer, Pistolet maszynowy, Jednoręczna, Kompaktowa.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve">Ślepy ostrzał
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve"> Za każdy poziom tej umiejętności, zwiększ przyrost zasięgu z biodra o 2m dla broni z którąś z zasad Pistolet, Rewolwer, Pistolet maszynowy, Jednoręczna, Kompaktowa. </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Umiejetnosc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dobycie broni</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Predyspozycje</t>
+  </si>
+  <si>
     <t xml:space="preserve">Karabiny</t>
   </si>
   <si>
@@ -38,6 +112,11 @@
   </si>
   <si>
     <t xml:space="preserve">obsluga broni, refleks, strzelectwo, zmysl bitewny, ukrywanie, zreczne palce </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Broń awaryjna w walce wręcz
+W walce wręcz zamiast ataku możesz strzelać z broni z zasadą Pistolet, Rewolwer, Pistolet maszynowy, Jednoręczna, Kompaktowa. Zwiększasz odrzut podwójnie. Ten strzał musi być wykonany z modyfikatorem „Z biodra”. Używasz wtedy poziomu tej umiejętności jako poziomu kości ataku (nie sumuje się z Wprawą).  
+Jest chujowa - po reworku walki wrecz jest bardzo słabo (chociazby zeby nie zamieniac kosci ataku na poziom tego skilla)</t>
   </si>
   <si>
     <t xml:space="preserve">Karabiny maszynowe</t>
@@ -185,7 +264,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -226,6 +305,13 @@
     </font>
     <font>
       <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <b val="true"/>
       <sz val="11"/>
       <name val="Times New Roman"/>
       <family val="1"/>
@@ -277,7 +363,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -290,7 +376,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -312,227 +414,323 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:Q27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="L4" activeCellId="0" sqref="L4:M4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="131.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="44.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="20.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="24.17"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="152.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
+      <c r="A3" s="0" t="s">
+        <v>20</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>21</v>
+      </c>
+      <c r="G3" s="6"/>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" customFormat="false" ht="135.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="8.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="8.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3" t="s">
-        <v>34</v>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>51</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
-        <v>36</v>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="7" t="s">
+        <v>53</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="3" t="s">
-        <v>44</v>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="s">
-        <v>46</v>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="7" t="s">
+        <v>63</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>48</v>
+        <v>65</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
-        <v>50</v>
+      <c r="A26" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>51</v>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="N4:Q4"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
jezyki zrobione, wraz z testem
</commit_message>
<xml_diff>
--- a/Specjalizacje.xlsx
+++ b/Specjalizacje.xlsx
@@ -363,7 +363,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -390,6 +390,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -416,17 +420,20 @@
   </sheetPr>
   <dimension ref="A1:Q27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L4" activeCellId="0" sqref="L4:M4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N4" activeCellId="0" sqref="N4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="131.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="44.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="11.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="20.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="24.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="9" style="0" width="11.59"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -536,12 +543,12 @@
       </c>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
-      <c r="N4" s="3" t="s">
+      <c r="N4" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="3"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
@@ -656,7 +663,7 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="8" t="s">
         <v>53</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -696,7 +703,7 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="7" t="s">
+      <c r="A24" s="8" t="s">
         <v>63</v>
       </c>
       <c r="B24" s="1" t="s">

</xml_diff>